<commit_message>
changed colors, noted to-dos, fixed bugs
</commit_message>
<xml_diff>
--- a/documentation/defect_tracking_tool.xlsx
+++ b/documentation/defect_tracking_tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgan.e.marino/Documents/GitHub/EECS448_Project3/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{682C7907-0AE0-D745-9436-1B5DF58F6327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66BB476-379A-F24F-B194-ED49544B16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13560" yWindow="500" windowWidth="15240" windowHeight="15780" xr2:uid="{6DEB9BFA-B066-CB48-804A-F84C30982553}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>DEFECT TRACKING TOOL</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Description of Fix</t>
+  </si>
+  <si>
+    <t>11.02.2021</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Pressed R,D in quick succession and snake went up, then no controls worked until the game was over</t>
+  </si>
+  <si>
+    <t>Due to the fact that the gridding is off for food and snake navigation, snake would eat food that was at least 1 snake width away from the snake. Need to work on accuracy and making the game a consistent square grid?</t>
   </si>
 </sst>
 </file>
@@ -421,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3437B5-3F3B-7240-975A-F1C78888FCD9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,6 +475,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>